<commit_message>
working grid and cartogram
</commit_message>
<xml_diff>
--- a/admin/india_states_meta.xlsx
+++ b/admin/india_states_meta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/U6105158/Sites/chart-module-india-carto/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{587ABBB1-F60B-814D-80B1-83685DC74ABB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5316707E-AF04-1C44-A3E2-F5366A6512BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16840" xr2:uid="{62085680-A67C-BE4B-90EF-6A7542FAD079}"/>
+    <workbookView xWindow="-1460" yWindow="-25160" windowWidth="32740" windowHeight="24500" xr2:uid="{62085680-A67C-BE4B-90EF-6A7542FAD079}"/>
   </bookViews>
   <sheets>
     <sheet name="india_states_meta" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="123">
   <si>
     <t>AN</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Andaman and Nicobar Islands</t>
   </si>
   <si>
-    <t>AP</t>
-  </si>
-  <si>
     <t>Andhra Pradesh</t>
   </si>
   <si>
@@ -408,15 +405,16 @@
     <t>Egypt</t>
   </si>
   <si>
-    <t>X</t>
+    <t>ii</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -468,7 +466,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -476,6 +474,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -791,528 +790,678 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69C978F-EE86-5147-8C69-8A9299704FEF}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D35" sqref="D35:D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="37.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" t="s">
         <v>72</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" t="s">
         <v>73</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>76</v>
       </c>
       <c r="E1" t="s">
         <v>74</v>
       </c>
-      <c r="F1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="6">
+      <c r="C2" s="6">
         <v>417036</v>
+      </c>
+      <c r="D2">
+        <v>7</v>
       </c>
       <c r="E2">
         <v>7</v>
       </c>
-      <c r="F2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="6">
-        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!C3, Sheet2!A:A,0))</f>
+      <c r="C3" s="6">
+        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B3, Sheet2!A:A,0))</f>
         <v>53903393</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
       </c>
       <c r="E3">
         <v>5</v>
       </c>
-      <c r="F3">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="6">
+        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B4, Sheet2!A:A,0))</f>
+        <v>1570458</v>
+      </c>
+      <c r="D4">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="6">
+        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B5, Sheet2!A:A,0))</f>
+        <v>35607039</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="6">
+        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B6, Sheet2!A:A,0))</f>
+        <v>124799926</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="6">
+        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B7, Sheet2!A:A,0))</f>
+        <v>1158473</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="6">
+        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B8, Sheet2!A:A,0))</f>
+        <v>29436231</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>123</v>
-      </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="6">
+        <v>615724</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
         <v>5</v>
       </c>
-      <c r="D4" s="6">
-        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!C4, Sheet2!A:A,0))</f>
-        <v>1570458</v>
-      </c>
-      <c r="E4">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="6">
+        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B10, Sheet2!A:A,0))</f>
+        <v>18710922</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="6">
+        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B11, Sheet2!A:A,0))</f>
+        <v>1586250</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="6">
+        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B12, Sheet2!A:A,0))</f>
+        <v>63872399</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="6">
+        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B13, Sheet2!A:A,0))</f>
+        <v>28204692</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="6">
+        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B14, Sheet2!A:A,0))</f>
+        <v>7451955</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="6">
+        <v>13606320</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="6">
+        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B16, Sheet2!A:A,0))</f>
+        <v>38593948</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="6">
+        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B17, Sheet2!A:A,0))</f>
+        <v>67562686</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="6">
+        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B18, Sheet2!A:A,0))</f>
+        <v>35699443</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="6">
+        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B19, Sheet2!A:A,0))</f>
+        <v>289023</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="6">
+        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B20, Sheet2!A:A,0))</f>
+        <v>73183</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="6">
+        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B21, Sheet2!A:A,0))</f>
+        <v>85358965</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="6">
+        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B22, Sheet2!A:A,0))</f>
+        <v>123144223</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="6">
+        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B23, Sheet2!A:A,0))</f>
+        <v>3091545</v>
+      </c>
+      <c r="D23">
         <v>9</v>
       </c>
-      <c r="F4">
+      <c r="E23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="6">
+        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B24, Sheet2!A:A,0))</f>
+        <v>3366710</v>
+      </c>
+      <c r="D24">
+        <v>8</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="6">
+        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B25, Sheet2!A:A,0))</f>
+        <v>1239244</v>
+      </c>
+      <c r="D25">
+        <v>9</v>
+      </c>
+      <c r="E25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="6">
+        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B26, Sheet2!A:A,0))</f>
+        <v>2249695</v>
+      </c>
+      <c r="D26">
+        <v>8</v>
+      </c>
+      <c r="E26">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="6">
+        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B27, Sheet2!A:A,0))</f>
+        <v>46356334</v>
+      </c>
+      <c r="D27">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="E27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="6">
+        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B28, Sheet2!A:A,0))</f>
+        <v>1413542</v>
+      </c>
+      <c r="D28">
+        <v>5</v>
+      </c>
+      <c r="E28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="6">
+        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B29, Sheet2!A:A,0))</f>
+        <v>30141373</v>
+      </c>
+      <c r="D29">
+        <v>3</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="6">
+        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B30, Sheet2!A:A,0))</f>
+        <v>81032689</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="6">
+        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B31, Sheet2!A:A,0))</f>
+        <v>690251</v>
+      </c>
+      <c r="D31">
         <v>7</v>
       </c>
-      <c r="D5" s="6">
-        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!C5, Sheet2!A:A,0))</f>
-        <v>35607039</v>
-      </c>
-      <c r="E5">
+      <c r="E31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="6">
+        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B32, Sheet2!A:A,0))</f>
+        <v>77841267</v>
+      </c>
+      <c r="D32">
+        <v>4</v>
+      </c>
+      <c r="E32">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="6">
+        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B33, Sheet2!A:A,0))</f>
+        <v>38510982</v>
+      </c>
+      <c r="D33">
+        <v>4</v>
+      </c>
+      <c r="E33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="6">
+        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B34, Sheet2!A:A,0))</f>
+        <v>4169794</v>
+      </c>
+      <c r="D34">
+        <v>8</v>
+      </c>
+      <c r="E34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" s="6">
+        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B35, Sheet2!A:A,0))</f>
+        <v>237882725</v>
+      </c>
+      <c r="D35">
+        <v>5</v>
+      </c>
+      <c r="E35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="6">
+        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B36, Sheet2!A:A,0))</f>
+        <v>11250858</v>
+      </c>
+      <c r="D36">
+        <v>4</v>
+      </c>
+      <c r="E36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" s="6">
+        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B37, Sheet2!A:A,0))</f>
+        <v>99609303</v>
+      </c>
+      <c r="D37">
         <v>7</v>
       </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>123</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="6">
-        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!C6, Sheet2!A:A,0))</f>
-        <v>124799926</v>
-      </c>
-      <c r="E6">
-        <v>6</v>
-      </c>
-      <c r="F6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>123</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="6">
-        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!C7, Sheet2!A:A,0))</f>
-        <v>1158473</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="6">
-        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!C8, Sheet2!A:A,0))</f>
-        <v>29436231</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="6">
-        <v>615724</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="6">
-        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!C10, Sheet2!A:A,0))</f>
-        <v>18710922</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
-        <v>123</v>
-      </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="6">
-        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!C11, Sheet2!A:A,0))</f>
-        <v>1586250</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" t="s">
-        <v>123</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="6">
-        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!C12, Sheet2!A:A,0))</f>
-        <v>63872399</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" t="s">
-        <v>123</v>
-      </c>
-      <c r="C13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="6">
-        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!C13, Sheet2!A:A,0))</f>
-        <v>28204692</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" t="s">
-        <v>123</v>
-      </c>
-      <c r="C14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="6">
-        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!C14, Sheet2!A:A,0))</f>
-        <v>7451955</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" t="s">
-        <v>123</v>
-      </c>
-      <c r="C15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="6">
-        <v>13606320</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" t="s">
-        <v>123</v>
-      </c>
-      <c r="C16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="6">
-        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!C16, Sheet2!A:A,0))</f>
-        <v>38593948</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="6">
-        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!C17, Sheet2!A:A,0))</f>
-        <v>67562686</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="6">
-        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!C18, Sheet2!A:A,0))</f>
-        <v>35699443</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="6">
-        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!C19, Sheet2!A:A,0))</f>
-        <v>289023</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="6">
-        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!C20, Sheet2!A:A,0))</f>
-        <v>73183</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="6">
-        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!C21, Sheet2!A:A,0))</f>
-        <v>85358965</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" s="6">
-        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!C22, Sheet2!A:A,0))</f>
-        <v>123144223</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" s="6">
-        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!C23, Sheet2!A:A,0))</f>
-        <v>3091545</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="6">
-        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!C24, Sheet2!A:A,0))</f>
-        <v>3366710</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="6">
-        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!C25, Sheet2!A:A,0))</f>
-        <v>1239244</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" t="s">
-        <v>49</v>
-      </c>
-      <c r="D26" s="6">
-        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!C26, Sheet2!A:A,0))</f>
-        <v>2249695</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27" s="6">
-        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!C27, Sheet2!A:A,0))</f>
-        <v>46356334</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>52</v>
-      </c>
-      <c r="C28" t="s">
-        <v>53</v>
-      </c>
-      <c r="D28" s="6">
-        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!C28, Sheet2!A:A,0))</f>
-        <v>1413542</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" t="s">
-        <v>55</v>
-      </c>
-      <c r="D29" s="6">
-        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!C29, Sheet2!A:A,0))</f>
-        <v>30141373</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>56</v>
-      </c>
-      <c r="C30" t="s">
-        <v>57</v>
-      </c>
-      <c r="D30" s="6">
-        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!C30, Sheet2!A:A,0))</f>
-        <v>81032689</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>58</v>
-      </c>
-      <c r="C31" t="s">
-        <v>59</v>
-      </c>
-      <c r="D31" s="6">
-        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!C31, Sheet2!A:A,0))</f>
-        <v>690251</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>60</v>
-      </c>
-      <c r="C32" t="s">
-        <v>61</v>
-      </c>
-      <c r="D32" s="6">
-        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!C32, Sheet2!A:A,0))</f>
-        <v>77841267</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>62</v>
-      </c>
-      <c r="C33" t="s">
-        <v>63</v>
-      </c>
-      <c r="D33" s="6">
-        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!C33, Sheet2!A:A,0))</f>
-        <v>38510982</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>64</v>
-      </c>
-      <c r="C34" t="s">
-        <v>65</v>
-      </c>
-      <c r="D34" s="6">
-        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!C34, Sheet2!A:A,0))</f>
-        <v>4169794</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>66</v>
-      </c>
-      <c r="C35" t="s">
-        <v>67</v>
-      </c>
-      <c r="D35" s="6">
-        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!C35, Sheet2!A:A,0))</f>
-        <v>237882725</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>68</v>
-      </c>
-      <c r="C36" t="s">
-        <v>69</v>
-      </c>
-      <c r="D36" s="6">
-        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!C36, Sheet2!A:A,0))</f>
-        <v>11250858</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>70</v>
-      </c>
-      <c r="C37" t="s">
-        <v>71</v>
-      </c>
-      <c r="D37" s="6">
-        <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!C37, Sheet2!A:A,0))</f>
-        <v>99609303</v>
+      <c r="E37">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1348,15 +1497,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2">
         <v>417036</v>
@@ -1364,7 +1513,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>53903393</v>
@@ -1372,7 +1521,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>1570458</v>
@@ -1380,7 +1529,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>35607039</v>
@@ -1388,7 +1537,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>124799926</v>
@@ -1396,7 +1545,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>1158473</v>
@@ -1404,7 +1553,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>29436231</v>
@@ -1412,7 +1561,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B9">
         <v>615724</v>
@@ -1420,7 +1569,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10">
         <v>18710922</v>
@@ -1428,7 +1577,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11">
         <v>1586250</v>
@@ -1436,7 +1585,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12">
         <v>63872399</v>
@@ -1444,7 +1593,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13">
         <v>28204692</v>
@@ -1452,7 +1601,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14">
         <v>7451955</v>
@@ -1460,7 +1609,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B15">
         <v>13606320</v>
@@ -1468,7 +1617,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16">
         <v>38593948</v>
@@ -1476,7 +1625,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17">
         <v>67562686</v>
@@ -1484,7 +1633,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18">
         <v>35699443</v>
@@ -1492,7 +1641,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19">
         <v>289023</v>
@@ -1500,7 +1649,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20">
         <v>73183</v>
@@ -1508,7 +1657,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21">
         <v>85358965</v>
@@ -1516,7 +1665,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22">
         <v>123144223</v>
@@ -1524,7 +1673,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B23">
         <v>3091545</v>
@@ -1532,7 +1681,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24">
         <v>3366710</v>
@@ -1540,7 +1689,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B25">
         <v>1239244</v>
@@ -1548,7 +1697,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B26">
         <v>2249695</v>
@@ -1556,7 +1705,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B27">
         <v>46356334</v>
@@ -1564,7 +1713,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B28">
         <v>1413542</v>
@@ -1572,7 +1721,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B29">
         <v>30141373</v>
@@ -1580,7 +1729,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B30">
         <v>81032689</v>
@@ -1588,7 +1737,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B31">
         <v>690251</v>
@@ -1596,7 +1745,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B32">
         <v>77841267</v>
@@ -1604,7 +1753,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B33">
         <v>38510982</v>
@@ -1612,7 +1761,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B34">
         <v>4169794</v>
@@ -1620,7 +1769,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B35">
         <v>237882725</v>
@@ -1628,7 +1777,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B36">
         <v>11250858</v>
@@ -1636,7 +1785,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B37">
         <v>99609303</v>
@@ -1664,10 +1813,10 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>82</v>
       </c>
       <c r="C1" s="5">
         <v>417036</v>
@@ -1685,7 +1834,7 @@
         <v>0.03</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I1" s="4">
         <v>176</v>
@@ -1696,7 +1845,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="5">
         <v>53903393</v>
@@ -1714,7 +1863,7 @@
         <v>3.93</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I2" s="4">
         <v>27</v>
@@ -1725,7 +1874,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="5">
         <v>1570458</v>
@@ -1743,7 +1892,7 @@
         <v>0.11</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I3" s="4">
         <v>153</v>
@@ -1754,7 +1903,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="5">
         <v>35607039</v>
@@ -1772,7 +1921,7 @@
         <v>2.6</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I4" s="4">
         <v>41</v>
@@ -1783,7 +1932,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="5">
         <v>124799926</v>
@@ -1801,7 +1950,7 @@
         <v>9.1</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I5" s="4">
         <v>12</v>
@@ -1809,10 +1958,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="5">
         <v>1158473</v>
@@ -1830,7 +1979,7 @@
         <v>0.08</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I6" s="4">
         <v>159</v>
@@ -1841,7 +1990,7 @@
         <v>17</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="5">
         <v>29436231</v>
@@ -1859,7 +2008,7 @@
         <v>2.15</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I7" s="4">
         <v>48</v>
@@ -1867,10 +2016,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C8" s="5">
         <v>615724</v>
@@ -1888,7 +2037,7 @@
         <v>0.04</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I8" s="4">
         <v>170</v>
@@ -1896,10 +2045,10 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="5">
         <v>18710922</v>
@@ -1917,7 +2066,7 @@
         <v>1.36</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I9" s="4">
         <v>63</v>
@@ -1928,7 +2077,7 @@
         <v>25</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="5">
         <v>1586250</v>
@@ -1946,7 +2095,7 @@
         <v>0.12</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I10" s="4">
         <v>153</v>
@@ -1957,7 +2106,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="5">
         <v>63872399</v>
@@ -1975,7 +2124,7 @@
         <v>4.66</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I11" s="4">
         <v>23</v>
@@ -1986,7 +2135,7 @@
         <v>18</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="5">
         <v>28204692</v>
@@ -2004,7 +2153,7 @@
         <v>2.06</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I12" s="4">
         <v>51</v>
@@ -2015,7 +2164,7 @@
         <v>20</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="5">
         <v>7451955</v>
@@ -2033,7 +2182,7 @@
         <v>0.54</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I13" s="4">
         <v>104</v>
@@ -2041,10 +2190,10 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>98</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>99</v>
       </c>
       <c r="C14" s="5">
         <v>13606320</v>
@@ -2062,7 +2211,7 @@
         <v>0.99</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I14" s="4">
         <v>75</v>
@@ -2073,7 +2222,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" s="5">
         <v>38593948</v>
@@ -2091,7 +2240,7 @@
         <v>2.81</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I15" s="4">
         <v>37</v>
@@ -2102,7 +2251,7 @@
         <v>8</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" s="5">
         <v>67562686</v>
@@ -2120,7 +2269,7 @@
         <v>4.93</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I16" s="4">
         <v>21</v>
@@ -2131,7 +2280,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="5">
         <v>35699443</v>
@@ -2149,7 +2298,7 @@
         <v>2.6</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I17" s="4">
         <v>41</v>
@@ -2157,10 +2306,10 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="5">
         <v>289023</v>
@@ -2178,7 +2327,7 @@
         <v>0.02</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I18" s="4">
         <v>183</v>
@@ -2186,10 +2335,10 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" s="5">
         <v>73183</v>
@@ -2207,7 +2356,7 @@
         <v>0.01</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I19" s="4">
         <v>204</v>
@@ -2218,7 +2367,7 @@
         <v>5</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20" s="5">
         <v>85358965</v>
@@ -2236,7 +2385,7 @@
         <v>6.22</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I20" s="4">
         <v>17</v>
@@ -2247,7 +2396,7 @@
         <v>3</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21" s="5">
         <v>123144223</v>
@@ -2265,7 +2414,7 @@
         <v>8.98</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I21" s="4">
         <v>12</v>
@@ -2276,7 +2425,7 @@
         <v>23</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C22" s="5">
         <v>3091545</v>
@@ -2294,7 +2443,7 @@
         <v>0.23</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I22" s="4">
         <v>137</v>
@@ -2305,7 +2454,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C23" s="5">
         <v>3366710</v>
@@ -2323,7 +2472,7 @@
         <v>0.25</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I23" s="4">
         <v>135</v>
@@ -2334,7 +2483,7 @@
         <v>27</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C24" s="5">
         <v>1239244</v>
@@ -2352,7 +2501,7 @@
         <v>0.09</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I24" s="4">
         <v>158</v>
@@ -2363,7 +2512,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C25" s="5">
         <v>2249695</v>
@@ -2381,7 +2530,7 @@
         <v>0.16</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I25" s="4">
         <v>146</v>
@@ -2392,7 +2541,7 @@
         <v>11</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C26" s="5">
         <v>46356334</v>
@@ -2410,7 +2559,7 @@
         <v>3.38</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I26" s="4">
         <v>31</v>
@@ -2418,10 +2567,10 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C27" s="5">
         <v>1413542</v>
@@ -2439,7 +2588,7 @@
         <v>0.1</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I27" s="4">
         <v>153</v>
@@ -2450,7 +2599,7 @@
         <v>16</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" s="5">
         <v>30141373</v>
@@ -2468,7 +2617,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I28" s="4">
         <v>48</v>
@@ -2479,7 +2628,7 @@
         <v>6</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C29" s="5">
         <v>81032689</v>
@@ -2497,7 +2646,7 @@
         <v>5.91</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I29" s="4">
         <v>20</v>
@@ -2508,7 +2657,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C30" s="5">
         <v>690251</v>
@@ -2526,7 +2675,7 @@
         <v>0.05</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I30" s="4">
         <v>166</v>
@@ -2537,7 +2686,7 @@
         <v>7</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C31" s="5">
         <v>77841267</v>
@@ -2555,7 +2704,7 @@
         <v>5.68</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I31" s="4">
         <v>20</v>
@@ -2566,7 +2715,7 @@
         <v>12</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C32" s="5">
         <v>39362732</v>
@@ -2584,7 +2733,7 @@
         <v>2.87</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I32" s="4">
         <v>36</v>
@@ -2595,7 +2744,7 @@
         <v>21</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C33" s="5">
         <v>4169794</v>
@@ -2613,7 +2762,7 @@
         <v>0.3</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I33" s="4">
         <v>130</v>
@@ -2624,7 +2773,7 @@
         <v>1</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C34" s="5">
         <v>237882725</v>
@@ -2642,7 +2791,7 @@
         <v>17.350000000000001</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I34" s="4">
         <v>5</v>
@@ -2653,7 +2802,7 @@
         <v>19</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C35" s="5">
         <v>11250858</v>
@@ -2671,7 +2820,7 @@
         <v>0.82</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I35" s="4">
         <v>84</v>
@@ -2682,7 +2831,7 @@
         <v>4</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C36" s="5">
         <v>99609303</v>
@@ -2700,7 +2849,7 @@
         <v>7.26</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I36" s="4">
         <v>15</v>

</xml_diff>

<commit_message>
added short names and narrowed grid to 8 columns.
</commit_message>
<xml_diff>
--- a/admin/india_states_meta.xlsx
+++ b/admin/india_states_meta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/U6105158/Sites/chart-module-india-carto/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5316707E-AF04-1C44-A3E2-F5366A6512BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B52FF1-2370-D948-98E4-EB9DE440E638}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1460" yWindow="-25160" windowWidth="32740" windowHeight="24500" xr2:uid="{62085680-A67C-BE4B-90EF-6A7542FAD079}"/>
+    <workbookView xWindow="18760" yWindow="-24680" windowWidth="32740" windowHeight="24500" xr2:uid="{62085680-A67C-BE4B-90EF-6A7542FAD079}"/>
   </bookViews>
   <sheets>
     <sheet name="india_states_meta" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="130">
   <si>
     <t>AN</t>
   </si>
@@ -406,6 +406,27 @@
   </si>
   <si>
     <t>ii</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
+    <t>DNH/DD</t>
+  </si>
+  <si>
+    <t>Andhra Pr.</t>
+  </si>
+  <si>
+    <t>Arunachal Pr.</t>
+  </si>
+  <si>
+    <t>Himachal Pr.</t>
+  </si>
+  <si>
+    <t>Madhya Pr.</t>
+  </si>
+  <si>
+    <t>Uttar Pr.</t>
   </si>
 </sst>
 </file>
@@ -414,7 +435,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -474,7 +495,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -790,682 +811,795 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69C978F-EE86-5147-8C69-8A9299704FEF}">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35:D36"/>
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="37.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>71</v>
       </c>
       <c r="B1" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" t="s">
         <v>75</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>73</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="6">
         <v>417036</v>
-      </c>
-      <c r="D2">
-        <v>7</v>
       </c>
       <c r="E2">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>122</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" s="6">
         <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B3, Sheet2!A:A,0))</f>
         <v>53903393</v>
       </c>
-      <c r="D3">
-        <v>5</v>
-      </c>
       <c r="E3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D4" s="6">
         <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B4, Sheet2!A:A,0))</f>
         <v>1570458</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>9</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="6">
         <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B5, Sheet2!A:A,0))</f>
         <v>35607039</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>7</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="6">
         <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B6, Sheet2!A:A,0))</f>
         <v>124799926</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>6</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="6">
         <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B7, Sheet2!A:A,0))</f>
         <v>1158473</v>
       </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
       <c r="E7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="6">
         <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B8, Sheet2!A:A,0))</f>
         <v>29436231</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>5</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D9" s="6">
         <v>615724</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>2</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="6">
         <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B10, Sheet2!A:A,0))</f>
         <v>18710922</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>3</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
       <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="6">
         <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B11, Sheet2!A:A,0))</f>
         <v>1586250</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>3</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>19</v>
       </c>
       <c r="B12" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="6">
         <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B12, Sheet2!A:A,0))</f>
         <v>63872399</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>1</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>21</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="6">
         <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B13, Sheet2!A:A,0))</f>
         <v>28204692</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>2</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>23</v>
       </c>
       <c r="B14" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" t="s">
+        <v>127</v>
+      </c>
+      <c r="D14" s="6">
         <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B14, Sheet2!A:A,0))</f>
         <v>7451955</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>4</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>25</v>
       </c>
       <c r="B15" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" s="6">
         <v>13606320</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>3</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>27</v>
       </c>
       <c r="B16" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="6">
         <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B16, Sheet2!A:A,0))</f>
         <v>38593948</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>6</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>29</v>
       </c>
       <c r="B17" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="6">
         <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B17, Sheet2!A:A,0))</f>
         <v>67562686</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>4</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>31</v>
       </c>
       <c r="B18" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="6">
         <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B18, Sheet2!A:A,0))</f>
         <v>35699443</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>4</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>33</v>
       </c>
       <c r="B19" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="6">
         <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B19, Sheet2!A:A,0))</f>
         <v>289023</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>4</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>35</v>
       </c>
       <c r="B20" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="6">
         <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B20, Sheet2!A:A,0))</f>
         <v>73183</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>3</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>37</v>
       </c>
       <c r="B21" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" t="s">
+        <v>128</v>
+      </c>
+      <c r="D21" s="6">
         <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B21, Sheet2!A:A,0))</f>
         <v>85358965</v>
       </c>
-      <c r="D21">
-        <v>4</v>
-      </c>
       <c r="E21">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>39</v>
       </c>
       <c r="B22" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="6">
         <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B22, Sheet2!A:A,0))</f>
         <v>123144223</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>3</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>41</v>
       </c>
       <c r="B23" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="6">
         <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B23, Sheet2!A:A,0))</f>
         <v>3091545</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>9</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>43</v>
       </c>
       <c r="B24" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="6">
         <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B24, Sheet2!A:A,0))</f>
         <v>3366710</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>8</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>45</v>
       </c>
       <c r="B25" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="6">
         <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B25, Sheet2!A:A,0))</f>
         <v>1239244</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>9</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>47</v>
       </c>
       <c r="B26" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="6">
         <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B26, Sheet2!A:A,0))</f>
         <v>2249695</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>8</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>49</v>
       </c>
       <c r="B27" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="6">
         <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B27, Sheet2!A:A,0))</f>
         <v>46356334</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>6</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>51</v>
       </c>
       <c r="B28" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="6">
         <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B28, Sheet2!A:A,0))</f>
         <v>1413542</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>5</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>53</v>
       </c>
       <c r="B29" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="6">
         <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B29, Sheet2!A:A,0))</f>
         <v>30141373</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <v>3</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>55</v>
       </c>
       <c r="B30" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" s="6">
         <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B30, Sheet2!A:A,0))</f>
         <v>81032689</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>2</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>57</v>
       </c>
       <c r="B31" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" s="6">
         <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B31, Sheet2!A:A,0))</f>
         <v>690251</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <v>7</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>59</v>
       </c>
       <c r="B32" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C32" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="6">
         <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B32, Sheet2!A:A,0))</f>
         <v>77841267</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <v>4</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>61</v>
       </c>
       <c r="B33" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C33" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" s="6">
         <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B33, Sheet2!A:A,0))</f>
         <v>38510982</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>4</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>63</v>
       </c>
       <c r="B34" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C34" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" s="6">
         <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B34, Sheet2!A:A,0))</f>
         <v>4169794</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>8</v>
       </c>
-      <c r="E34">
+      <c r="F34">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>65</v>
       </c>
       <c r="B35" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="6">
+      <c r="C35" t="s">
+        <v>129</v>
+      </c>
+      <c r="D35" s="6">
         <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B35, Sheet2!A:A,0))</f>
         <v>237882725</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <v>5</v>
       </c>
-      <c r="E35">
+      <c r="F35">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>67</v>
       </c>
       <c r="B36" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C36" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" s="6">
         <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B36, Sheet2!A:A,0))</f>
         <v>11250858</v>
       </c>
-      <c r="D36">
+      <c r="E36">
         <v>4</v>
       </c>
-      <c r="E36">
+      <c r="F36">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>69</v>
       </c>
       <c r="B37" t="s">
         <v>70</v>
       </c>
-      <c r="C37" s="6">
+      <c r="C37" t="s">
+        <v>70</v>
+      </c>
+      <c r="D37" s="6">
         <f>INDEX(Sheet2!B:B, MATCH(india_states_meta!B37, Sheet2!A:A,0))</f>
         <v>99609303</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <v>7</v>
       </c>
-      <c r="E37">
+      <c r="F37">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>